<commit_message>
Added list of work to be done
</commit_message>
<xml_diff>
--- a/LambdaExperimentWithDynamicArrays.xlsx
+++ b/LambdaExperimentWithDynamicArrays.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E534C36E-0D23-41DC-B928-CD1AF4017AF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC1FE65F-BA3F-41E3-BCAC-929AEBB6A99E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{79507A11-E329-490F-8F3D-C4CA49231C76}"/>
+    <workbookView xWindow="-26490" yWindow="2310" windowWidth="21600" windowHeight="11235" xr2:uid="{79507A11-E329-490F-8F3D-C4CA49231C76}"/>
   </bookViews>
   <sheets>
     <sheet name="Rayovac-Data" sheetId="1" r:id="rId1"/>
@@ -20,22 +20,22 @@
     <externalReference r:id="rId3"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_n24">'[2]2.4 GHz'!$A$2:$AC$106</definedName>
-    <definedName name="_n24NFMI">'[2]2.4 GHz + NFMI'!$A$2:$AC$91</definedName>
-    <definedName name="_nAgeFactor">'[1]Rechargeable-SOCs'!$C$7</definedName>
-    <definedName name="_nBat">[1]!_tZ[Z]</definedName>
-    <definedName name="_nBatType">[1]!_tBatType[BatType]</definedName>
-    <definedName name="_nDevice">[1]!_tConsol16[#All]</definedName>
-    <definedName name="_nGenesis">'[2]Genesis '!$A$2:$AC$48</definedName>
-    <definedName name="_nHeading">'[2]2.4 GHz + NFMI'!$A$1:$AC$1</definedName>
-    <definedName name="_nMatrix">[1]!_tMatrix[Matrix]</definedName>
-    <definedName name="_nProduct">[1]!_tProduct[Product]</definedName>
-    <definedName name="_nProgram">[1]!_tProgram[Program]</definedName>
-    <definedName name="_nVREF">[1]!_tVREF[VREF]</definedName>
-    <definedName name="_nWired">[2]Wired!$A$2:$AC$25</definedName>
-    <definedName name="_nWiredWireless">[1]!_tWiredWireless[Wired/2.4GHz]</definedName>
-    <definedName name="_tCur">[1]Scenarios!$H$69:$H$72</definedName>
-    <definedName name="_tTime">[1]Scenarios!$C$69:$F$77</definedName>
+    <definedName name="_n24">'[1]2.4 GHz'!$A$2:$AC$106</definedName>
+    <definedName name="_n24NFMI">'[1]2.4 GHz + NFMI'!$A$2:$AC$91</definedName>
+    <definedName name="_nAgeFactor">'[2]Rechargeable-SOCs'!$C$7</definedName>
+    <definedName name="_nBat">[2]!_tZ[Z]</definedName>
+    <definedName name="_nBatType">[2]!_tBatType[BatType]</definedName>
+    <definedName name="_nDevice">[2]!_tConsol16[#All]</definedName>
+    <definedName name="_nGenesis">'[1]Genesis '!$A$2:$AC$48</definedName>
+    <definedName name="_nHeading">'[1]2.4 GHz + NFMI'!$A$1:$AC$1</definedName>
+    <definedName name="_nMatrix">[2]!_tMatrix[Matrix]</definedName>
+    <definedName name="_nProduct">[2]!_tProduct[Product]</definedName>
+    <definedName name="_nProgram">[2]!_tProgram[Program]</definedName>
+    <definedName name="_nVREF">[2]!_tVREF[VREF]</definedName>
+    <definedName name="_nWired">[1]Wired!$A$2:$AC$25</definedName>
+    <definedName name="_nWiredWireless">[2]!_tWiredWireless[Wired/2.4GHz]</definedName>
+    <definedName name="_tCur">[2]Scenarios!$H$69:$H$72</definedName>
+    <definedName name="_tTime">[2]Scenarios!$C$69:$F$77</definedName>
     <definedName name="_X">'Rayovac-Data'!$B$91:$B$166</definedName>
     <definedName name="_Y">'Rayovac-Data'!$C$91:$C$166</definedName>
     <definedName name="dlint">_xlfn.LAMBDA(_xlpm.x,_xlpm.s,IF(_xlpm.x&lt;1,_xlpm.x,lint(_xlpm.s,_xlpm.x)))</definedName>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="26">
   <si>
     <t>Cht Ttl</t>
   </si>
@@ -162,6 +162,12 @@
   </si>
   <si>
     <t>Accu90</t>
+  </si>
+  <si>
+    <t>How to deal with the bump?</t>
+  </si>
+  <si>
+    <t>What is the "least surprising" approach?</t>
   </si>
 </sst>
 </file>
@@ -6511,2331 +6517,6 @@
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="DeviceCurrents"/>
-      <sheetName val="Revision-History"/>
-      <sheetName val="Data-Dictionary"/>
-      <sheetName val="Example-Pivot"/>
-      <sheetName val="Rechargeable-SOCs"/>
-      <sheetName val="Scenarios"/>
-      <sheetName val="Rayovac-Data"/>
-      <sheetName val="Logic"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4">
-        <row r="7">
-          <cell r="C7">
-            <v>0.8</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="5">
-        <row r="69">
-          <cell r="C69">
-            <v>0</v>
-          </cell>
-          <cell r="D69">
-            <v>3.5</v>
-          </cell>
-          <cell r="E69">
-            <v>0.16666666666666666</v>
-          </cell>
-          <cell r="F69">
-            <v>12.333333333333334</v>
-          </cell>
-          <cell r="H69">
-            <v>2700</v>
-          </cell>
-        </row>
-        <row r="70">
-          <cell r="C70">
-            <v>0.75</v>
-          </cell>
-          <cell r="D70">
-            <v>0</v>
-          </cell>
-          <cell r="E70">
-            <v>8.3333333333333329E-2</v>
-          </cell>
-          <cell r="F70">
-            <v>15.166666666666666</v>
-          </cell>
-          <cell r="H70">
-            <v>2430</v>
-          </cell>
-        </row>
-        <row r="71">
-          <cell r="C71">
-            <v>0</v>
-          </cell>
-          <cell r="D71">
-            <v>5</v>
-          </cell>
-          <cell r="E71">
-            <v>0.16666666666666666</v>
-          </cell>
-          <cell r="F71">
-            <v>12.833333333333332</v>
-          </cell>
-          <cell r="H71">
-            <v>1470</v>
-          </cell>
-        </row>
-        <row r="72">
-          <cell r="C72">
-            <v>1.5</v>
-          </cell>
-          <cell r="D72">
-            <v>0</v>
-          </cell>
-          <cell r="E72">
-            <v>8.3333333333333329E-2</v>
-          </cell>
-          <cell r="F72">
-            <v>16.416666666666668</v>
-          </cell>
-          <cell r="H72">
-            <v>1380</v>
-          </cell>
-        </row>
-        <row r="73">
-          <cell r="C73">
-            <v>13.833333333333334</v>
-          </cell>
-          <cell r="D73">
-            <v>0</v>
-          </cell>
-          <cell r="E73">
-            <v>0.16666666666666666</v>
-          </cell>
-          <cell r="F73">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="74">
-          <cell r="C74">
-            <v>15.833333333333334</v>
-          </cell>
-          <cell r="D74">
-            <v>0</v>
-          </cell>
-          <cell r="E74">
-            <v>0.16666666666666666</v>
-          </cell>
-          <cell r="F74">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="75">
-          <cell r="C75">
-            <v>0</v>
-          </cell>
-          <cell r="D75">
-            <v>3.5</v>
-          </cell>
-          <cell r="E75">
-            <v>0.16666666666666666</v>
-          </cell>
-          <cell r="F75">
-            <v>12.333333333333334</v>
-          </cell>
-        </row>
-        <row r="76">
-          <cell r="C76">
-            <v>0</v>
-          </cell>
-          <cell r="D76">
-            <v>5</v>
-          </cell>
-          <cell r="E76">
-            <v>0.16666666666666666</v>
-          </cell>
-          <cell r="F76">
-            <v>12.833333333333332</v>
-          </cell>
-        </row>
-        <row r="77">
-          <cell r="C77">
-            <v>0</v>
-          </cell>
-          <cell r="D77">
-            <v>0</v>
-          </cell>
-          <cell r="E77">
-            <v>0</v>
-          </cell>
-          <cell r="F77">
-            <v>16</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="6">
-        <row r="2">
-          <cell r="Q2" t="str">
-            <v>Derating vs Actual Current and Size</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="Q3" t="str">
-            <v>Actual Current (mA)</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="Q4" t="str">
-            <v>Derated Current (mA)</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="H7" t="str">
-            <v>10A</v>
-          </cell>
-          <cell r="J7" t="str">
-            <v>13</v>
-          </cell>
-          <cell r="L7" t="str">
-            <v>312</v>
-          </cell>
-          <cell r="N7" t="str">
-            <v>Surflink 10A</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="G9">
-            <v>1</v>
-          </cell>
-          <cell r="H9">
-            <v>1.1499999999999999</v>
-          </cell>
-          <cell r="I9">
-            <v>1</v>
-          </cell>
-          <cell r="J9">
-            <v>1.1000000000000001</v>
-          </cell>
-          <cell r="K9">
-            <v>1</v>
-          </cell>
-          <cell r="L9">
-            <v>1.1000000000000001</v>
-          </cell>
-          <cell r="M9">
-            <v>1</v>
-          </cell>
-          <cell r="N9">
-            <v>1.1499999999999999</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="G10">
-            <v>1.1000000000000001</v>
-          </cell>
-          <cell r="H10">
-            <v>1.2711277615384615</v>
-          </cell>
-          <cell r="I10">
-            <v>1.1000000000000001</v>
-          </cell>
-          <cell r="J10">
-            <v>1.2142652365853659</v>
-          </cell>
-          <cell r="K10">
-            <v>1.1000000000000001</v>
-          </cell>
-          <cell r="L10">
-            <v>1.2171137804878052</v>
-          </cell>
-          <cell r="M10">
-            <v>1.1000000000000001</v>
-          </cell>
-          <cell r="N10">
-            <v>1.2684635173913044</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="G11">
-            <v>1.2</v>
-          </cell>
-          <cell r="H11">
-            <v>1.3933696615384614</v>
-          </cell>
-          <cell r="I11">
-            <v>1.2</v>
-          </cell>
-          <cell r="J11">
-            <v>1.3293059707317072</v>
-          </cell>
-          <cell r="K11">
-            <v>1.2</v>
-          </cell>
-          <cell r="L11">
-            <v>1.3355209756097561</v>
-          </cell>
-          <cell r="M11">
-            <v>1.2</v>
-          </cell>
-          <cell r="N11">
-            <v>1.387556765217391</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="G12">
-            <v>1.3</v>
-          </cell>
-          <cell r="H12">
-            <v>1.5167257000000001</v>
-          </cell>
-          <cell r="I12">
-            <v>1.3</v>
-          </cell>
-          <cell r="J12">
-            <v>1.4451222024390245</v>
-          </cell>
-          <cell r="K12">
-            <v>1.3</v>
-          </cell>
-          <cell r="L12">
-            <v>1.4552215853658539</v>
-          </cell>
-          <cell r="M12">
-            <v>1.3</v>
-          </cell>
-          <cell r="N12">
-            <v>1.5072797434782608</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="G13">
-            <v>1.4</v>
-          </cell>
-          <cell r="H13">
-            <v>1.641195876923077</v>
-          </cell>
-          <cell r="I13">
-            <v>1.4</v>
-          </cell>
-          <cell r="J13">
-            <v>1.561713931707317</v>
-          </cell>
-          <cell r="K13">
-            <v>1.4</v>
-          </cell>
-          <cell r="L13">
-            <v>1.5762156097560975</v>
-          </cell>
-          <cell r="M13">
-            <v>1.4</v>
-          </cell>
-          <cell r="N13">
-            <v>1.6276324521739127</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="G14">
-            <v>1.5</v>
-          </cell>
-          <cell r="H14">
-            <v>1.7667801923076927</v>
-          </cell>
-          <cell r="I14">
-            <v>1.5</v>
-          </cell>
-          <cell r="J14">
-            <v>1.6790811585365855</v>
-          </cell>
-          <cell r="K14">
-            <v>1.5</v>
-          </cell>
-          <cell r="L14">
-            <v>1.6985030487804877</v>
-          </cell>
-          <cell r="M14">
-            <v>1.5</v>
-          </cell>
-          <cell r="N14">
-            <v>1.748614891304348</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="G15">
-            <v>1.6</v>
-          </cell>
-          <cell r="H15">
-            <v>1.8934786461538466</v>
-          </cell>
-          <cell r="I15">
-            <v>1.6</v>
-          </cell>
-          <cell r="J15">
-            <v>1.7972238829268292</v>
-          </cell>
-          <cell r="K15">
-            <v>1.6</v>
-          </cell>
-          <cell r="L15">
-            <v>1.8220839024390245</v>
-          </cell>
-          <cell r="M15">
-            <v>1.6</v>
-          </cell>
-          <cell r="N15">
-            <v>1.8702270608695652</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="G16">
-            <v>1.7</v>
-          </cell>
-          <cell r="H16">
-            <v>2.0212912384615387</v>
-          </cell>
-          <cell r="I16">
-            <v>1.7</v>
-          </cell>
-          <cell r="J16">
-            <v>1.9161421048780485</v>
-          </cell>
-          <cell r="K16">
-            <v>1.7</v>
-          </cell>
-          <cell r="L16">
-            <v>1.9469581707317072</v>
-          </cell>
-          <cell r="M16">
-            <v>1.7</v>
-          </cell>
-          <cell r="N16">
-            <v>1.9924689608695652</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="G17">
-            <v>1.8</v>
-          </cell>
-          <cell r="H17">
-            <v>2.1502179692307699</v>
-          </cell>
-          <cell r="I17">
-            <v>1.8</v>
-          </cell>
-          <cell r="J17">
-            <v>2.0358358243902441</v>
-          </cell>
-          <cell r="K17">
-            <v>1.8</v>
-          </cell>
-          <cell r="L17">
-            <v>2.0731258536585369</v>
-          </cell>
-          <cell r="M17">
-            <v>1.8</v>
-          </cell>
-          <cell r="N17">
-            <v>2.1153405913043479</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="G18">
-            <v>1.9</v>
-          </cell>
-          <cell r="H18">
-            <v>2.2802588384615392</v>
-          </cell>
-          <cell r="I18">
-            <v>1.9</v>
-          </cell>
-          <cell r="J18">
-            <v>2.1563050414634142</v>
-          </cell>
-          <cell r="K18">
-            <v>1.9</v>
-          </cell>
-          <cell r="L18">
-            <v>2.200586951219512</v>
-          </cell>
-          <cell r="M18">
-            <v>1.9</v>
-          </cell>
-          <cell r="N18">
-            <v>2.2388419521739129</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="G19">
-            <v>2</v>
-          </cell>
-          <cell r="H19">
-            <v>2.411413846153847</v>
-          </cell>
-          <cell r="I19">
-            <v>2</v>
-          </cell>
-          <cell r="J19">
-            <v>2.2775497560975606</v>
-          </cell>
-          <cell r="K19">
-            <v>2</v>
-          </cell>
-          <cell r="L19">
-            <v>2.3293414634146341</v>
-          </cell>
-          <cell r="M19">
-            <v>2</v>
-          </cell>
-          <cell r="N19">
-            <v>2.3629730434782612</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="G20">
-            <v>2.1</v>
-          </cell>
-          <cell r="H20">
-            <v>2.5436829923076929</v>
-          </cell>
-          <cell r="I20">
-            <v>2.1</v>
-          </cell>
-          <cell r="J20">
-            <v>2.399569968292683</v>
-          </cell>
-          <cell r="K20">
-            <v>2.1</v>
-          </cell>
-          <cell r="L20">
-            <v>2.4593893902439028</v>
-          </cell>
-          <cell r="M20">
-            <v>2.1</v>
-          </cell>
-          <cell r="N20">
-            <v>2.4877338652173919</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="G21">
-            <v>2.2000000000000002</v>
-          </cell>
-          <cell r="H21">
-            <v>2.6770662769230777</v>
-          </cell>
-          <cell r="I21">
-            <v>2.2000000000000002</v>
-          </cell>
-          <cell r="J21">
-            <v>2.5223656780487804</v>
-          </cell>
-          <cell r="K21">
-            <v>2.2000000000000002</v>
-          </cell>
-          <cell r="L21">
-            <v>2.5907307317073176</v>
-          </cell>
-          <cell r="M21">
-            <v>2.2000000000000002</v>
-          </cell>
-          <cell r="N21">
-            <v>2.6131244173913046</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="G22">
-            <v>2.2999999999999998</v>
-          </cell>
-          <cell r="H22">
-            <v>2.8115637000000007</v>
-          </cell>
-          <cell r="I22">
-            <v>2.2999999999999998</v>
-          </cell>
-          <cell r="J22">
-            <v>2.6459368853658529</v>
-          </cell>
-          <cell r="K22">
-            <v>2.2999999999999998</v>
-          </cell>
-          <cell r="L22">
-            <v>2.7233654878048781</v>
-          </cell>
-          <cell r="M22">
-            <v>2.2999999999999998</v>
-          </cell>
-          <cell r="N22">
-            <v>2.7391447000000002</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="G23">
-            <v>2.4</v>
-          </cell>
-          <cell r="H23">
-            <v>2.9423424000000002</v>
-          </cell>
-          <cell r="I23">
-            <v>2.4</v>
-          </cell>
-          <cell r="J23">
-            <v>2.7702835902439022</v>
-          </cell>
-          <cell r="K23">
-            <v>2.4</v>
-          </cell>
-          <cell r="L23">
-            <v>2.8572936585365856</v>
-          </cell>
-          <cell r="M23">
-            <v>2.4</v>
-          </cell>
-          <cell r="N23">
-            <v>2.8657947130434782</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="G24">
-            <v>2.5</v>
-          </cell>
-          <cell r="H24">
-            <v>3.0841875000000001</v>
-          </cell>
-          <cell r="I24">
-            <v>2.5</v>
-          </cell>
-          <cell r="J24">
-            <v>2.8954057926829262</v>
-          </cell>
-          <cell r="K24">
-            <v>2.5</v>
-          </cell>
-          <cell r="L24">
-            <v>2.9925152439024396</v>
-          </cell>
-          <cell r="M24">
-            <v>2.5</v>
-          </cell>
-          <cell r="N24">
-            <v>2.9930744565217395</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="G25">
-            <v>2.6</v>
-          </cell>
-          <cell r="H25">
-            <v>3.2383416000000014</v>
-          </cell>
-          <cell r="I25">
-            <v>2.6</v>
-          </cell>
-          <cell r="J25">
-            <v>3.0213034926829265</v>
-          </cell>
-          <cell r="K25">
-            <v>2.6</v>
-          </cell>
-          <cell r="L25">
-            <v>3.1290302439024393</v>
-          </cell>
-          <cell r="M25">
-            <v>2.6</v>
-          </cell>
-          <cell r="N25">
-            <v>3.1209839304347833</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="G26">
-            <v>2.7</v>
-          </cell>
-          <cell r="H26">
-            <v>3.4060473000000013</v>
-          </cell>
-          <cell r="I26">
-            <v>2.7</v>
-          </cell>
-          <cell r="J26">
-            <v>3.1479766902439024</v>
-          </cell>
-          <cell r="K26">
-            <v>2.7</v>
-          </cell>
-          <cell r="L26">
-            <v>3.2668386585365861</v>
-          </cell>
-          <cell r="M26">
-            <v>2.7</v>
-          </cell>
-          <cell r="N26">
-            <v>3.2495231347826095</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="G27">
-            <v>2.8</v>
-          </cell>
-          <cell r="H27">
-            <v>3.5885471999999998</v>
-          </cell>
-          <cell r="I27">
-            <v>2.8</v>
-          </cell>
-          <cell r="J27">
-            <v>3.2754253853658528</v>
-          </cell>
-          <cell r="K27">
-            <v>2.8</v>
-          </cell>
-          <cell r="L27">
-            <v>3.405940487804878</v>
-          </cell>
-          <cell r="M27">
-            <v>2.8</v>
-          </cell>
-          <cell r="N27">
-            <v>3.3786920695652181</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="G28">
-            <v>2.9</v>
-          </cell>
-          <cell r="H28">
-            <v>3.7870839000000003</v>
-          </cell>
-          <cell r="I28">
-            <v>2.9</v>
-          </cell>
-          <cell r="J28">
-            <v>3.4036495780487801</v>
-          </cell>
-          <cell r="K28">
-            <v>2.9</v>
-          </cell>
-          <cell r="L28">
-            <v>3.5463357317073174</v>
-          </cell>
-          <cell r="M28">
-            <v>2.9</v>
-          </cell>
-          <cell r="N28">
-            <v>3.5084907347826091</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="G29">
-            <v>3</v>
-          </cell>
-          <cell r="H29">
-            <v>4.0029000000000012</v>
-          </cell>
-          <cell r="I29">
-            <v>3</v>
-          </cell>
-          <cell r="J29">
-            <v>3.5326492682926824</v>
-          </cell>
-          <cell r="K29">
-            <v>3</v>
-          </cell>
-          <cell r="L29">
-            <v>3.6880243902439025</v>
-          </cell>
-          <cell r="M29">
-            <v>3</v>
-          </cell>
-          <cell r="N29">
-            <v>3.6389191304347834</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="G30">
-            <v>3.1</v>
-          </cell>
-          <cell r="H30">
-            <v>4.2372381000000017</v>
-          </cell>
-          <cell r="I30">
-            <v>3.1</v>
-          </cell>
-          <cell r="J30">
-            <v>3.6624244560975598</v>
-          </cell>
-          <cell r="K30">
-            <v>3.1</v>
-          </cell>
-          <cell r="L30">
-            <v>3.8310064634146346</v>
-          </cell>
-          <cell r="M30">
-            <v>3.1</v>
-          </cell>
-          <cell r="N30">
-            <v>3.7699772565217398</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="G31">
-            <v>3.2</v>
-          </cell>
-          <cell r="H31">
-            <v>4.4913408000000015</v>
-          </cell>
-          <cell r="I31">
-            <v>3.2</v>
-          </cell>
-          <cell r="J31">
-            <v>3.7929751414634141</v>
-          </cell>
-          <cell r="K31">
-            <v>3.2</v>
-          </cell>
-          <cell r="L31">
-            <v>3.9752819512195132</v>
-          </cell>
-          <cell r="M31">
-            <v>3.2</v>
-          </cell>
-          <cell r="N31">
-            <v>3.9016651130434798</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="G32">
-            <v>3.3</v>
-          </cell>
-          <cell r="H32">
-            <v>4.7664506999999992</v>
-          </cell>
-          <cell r="I32">
-            <v>3.3</v>
-          </cell>
-          <cell r="J32">
-            <v>3.9243013243902429</v>
-          </cell>
-          <cell r="K32">
-            <v>3.3</v>
-          </cell>
-          <cell r="L32">
-            <v>4.1208508536585366</v>
-          </cell>
-          <cell r="M32">
-            <v>3.3</v>
-          </cell>
-          <cell r="N32">
-            <v>4.033982700000001</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="G33">
-            <v>3.4</v>
-          </cell>
-          <cell r="H33">
-            <v>5.0638103999999986</v>
-          </cell>
-          <cell r="I33">
-            <v>3.4</v>
-          </cell>
-          <cell r="J33">
-            <v>4.0564030048780477</v>
-          </cell>
-          <cell r="K33">
-            <v>3.4</v>
-          </cell>
-          <cell r="L33">
-            <v>4.2677131707317084</v>
-          </cell>
-          <cell r="M33">
-            <v>3.4</v>
-          </cell>
-          <cell r="N33">
-            <v>4.1683184000000004</v>
-          </cell>
-          <cell r="Q33" t="str">
-            <v>312</v>
-          </cell>
-          <cell r="R33" t="str">
-            <v>13</v>
-          </cell>
-          <cell r="S33" t="str">
-            <v>10A</v>
-          </cell>
-          <cell r="T33" t="str">
-            <v>Surflink 10A</v>
-          </cell>
-          <cell r="U33" t="str">
-            <v>312</v>
-          </cell>
-          <cell r="V33" t="str">
-            <v>13</v>
-          </cell>
-          <cell r="W33" t="str">
-            <v>10A</v>
-          </cell>
-          <cell r="X33" t="str">
-            <v>Surflink 10A</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="G34">
-            <v>3.5</v>
-          </cell>
-          <cell r="H34">
-            <v>5.384662500000001</v>
-          </cell>
-          <cell r="I34">
-            <v>3.5</v>
-          </cell>
-          <cell r="J34">
-            <v>4.1892801829268285</v>
-          </cell>
-          <cell r="K34">
-            <v>3.5</v>
-          </cell>
-          <cell r="L34">
-            <v>4.4158689024390254</v>
-          </cell>
-          <cell r="M34">
-            <v>3.5</v>
-          </cell>
-          <cell r="N34">
-            <v>4.3178625000000004</v>
-          </cell>
-          <cell r="P34">
-            <v>0.1</v>
-          </cell>
-          <cell r="Q34">
-            <v>0.1</v>
-          </cell>
-          <cell r="R34">
-            <v>0.1</v>
-          </cell>
-          <cell r="S34">
-            <v>0.1</v>
-          </cell>
-          <cell r="T34">
-            <v>0.1</v>
-          </cell>
-          <cell r="U34" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="V34" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="W34" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="X34" t="e">
-            <v>#N/A</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="G35">
-            <v>3.6</v>
-          </cell>
-          <cell r="H35">
-            <v>5.7302496000000014</v>
-          </cell>
-          <cell r="I35">
-            <v>3.6</v>
-          </cell>
-          <cell r="J35">
-            <v>4.3229328585365838</v>
-          </cell>
-          <cell r="K35">
-            <v>3.6</v>
-          </cell>
-          <cell r="L35">
-            <v>4.5653180487804885</v>
-          </cell>
-          <cell r="M35">
-            <v>3.6</v>
-          </cell>
-          <cell r="N35">
-            <v>4.4838576000000021</v>
-          </cell>
-          <cell r="P35">
-            <v>0.4631578947368421</v>
-          </cell>
-          <cell r="Q35">
-            <v>0.4631578947368421</v>
-          </cell>
-          <cell r="R35">
-            <v>0.4631578947368421</v>
-          </cell>
-          <cell r="S35">
-            <v>0.4631578947368421</v>
-          </cell>
-          <cell r="T35">
-            <v>0.4631578947368421</v>
-          </cell>
-          <cell r="U35" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="V35" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="W35" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="X35" t="e">
-            <v>#N/A</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="G36">
-            <v>3.7</v>
-          </cell>
-          <cell r="H36">
-            <v>6.1018143000000009</v>
-          </cell>
-          <cell r="I36">
-            <v>3.7</v>
-          </cell>
-          <cell r="J36">
-            <v>4.4573610317073165</v>
-          </cell>
-          <cell r="K36">
-            <v>3.7</v>
-          </cell>
-          <cell r="L36">
-            <v>4.7160606097560986</v>
-          </cell>
-          <cell r="M36">
-            <v>3.7</v>
-          </cell>
-          <cell r="N36">
-            <v>4.6675463000000015</v>
-          </cell>
-          <cell r="P36">
-            <v>0.82631578947368423</v>
-          </cell>
-          <cell r="Q36">
-            <v>0.82631578947368423</v>
-          </cell>
-          <cell r="R36">
-            <v>0.82631578947368423</v>
-          </cell>
-          <cell r="S36">
-            <v>0.82631578947368423</v>
-          </cell>
-          <cell r="T36">
-            <v>0.82631578947368423</v>
-          </cell>
-          <cell r="U36" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="V36" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="W36" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="X36" t="e">
-            <v>#N/A</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="G37">
-            <v>3.8</v>
-          </cell>
-          <cell r="H37">
-            <v>6.5005992000000008</v>
-          </cell>
-          <cell r="I37">
-            <v>3.8</v>
-          </cell>
-          <cell r="J37">
-            <v>4.5925647024390228</v>
-          </cell>
-          <cell r="K37">
-            <v>3.8</v>
-          </cell>
-          <cell r="L37">
-            <v>4.868096585365854</v>
-          </cell>
-          <cell r="M37">
-            <v>3.8</v>
-          </cell>
-          <cell r="N37">
-            <v>4.8701711999999997</v>
-          </cell>
-          <cell r="P37">
-            <v>1.1894736842105265</v>
-          </cell>
-          <cell r="Q37">
-            <v>1.3230570603337615</v>
-          </cell>
-          <cell r="R37">
-            <v>1.3171964197689345</v>
-          </cell>
-          <cell r="S37">
-            <v>1.380502093117409</v>
-          </cell>
-          <cell r="T37">
-            <v>1.5350295401355334</v>
-          </cell>
-          <cell r="U37" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="V37" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="W37" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="X37" t="e">
-            <v>#N/A</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="G38">
-            <v>3.9</v>
-          </cell>
-          <cell r="H38">
-            <v>6.9278469000000014</v>
-          </cell>
-          <cell r="I38">
-            <v>3.9</v>
-          </cell>
-          <cell r="J38">
-            <v>4.7285438707317056</v>
-          </cell>
-          <cell r="K38">
-            <v>3.9</v>
-          </cell>
-          <cell r="L38">
-            <v>5.0214259756097572</v>
-          </cell>
-          <cell r="M38">
-            <v>3.9</v>
-          </cell>
-          <cell r="N38">
-            <v>5.0929749000000006</v>
-          </cell>
-          <cell r="P38">
-            <v>1.5526315789473686</v>
-          </cell>
-          <cell r="Q38">
-            <v>1.7635456033376125</v>
-          </cell>
-          <cell r="R38">
-            <v>1.7412615397946087</v>
-          </cell>
-          <cell r="S38">
-            <v>1.8334635890688264</v>
-          </cell>
-          <cell r="T38">
-            <v>2.0705484797601095</v>
-          </cell>
-          <cell r="U38" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="V38" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="W38" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="X38" t="e">
-            <v>#N/A</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="G39">
-            <v>4</v>
-          </cell>
-          <cell r="H39">
-            <v>7.3848000000000011</v>
-          </cell>
-          <cell r="I39">
-            <v>4</v>
-          </cell>
-          <cell r="J39">
-            <v>4.8652985365853647</v>
-          </cell>
-          <cell r="K39">
-            <v>4</v>
-          </cell>
-          <cell r="L39">
-            <v>5.1760487804878057</v>
-          </cell>
-          <cell r="M39">
-            <v>4</v>
-          </cell>
-          <cell r="N39">
-            <v>5.3372000000000019</v>
-          </cell>
-          <cell r="P39">
-            <v>1.9157894736842107</v>
-          </cell>
-          <cell r="Q39">
-            <v>2.2209166110397947</v>
-          </cell>
-          <cell r="R39">
-            <v>2.1754489437740694</v>
-          </cell>
-          <cell r="S39">
-            <v>2.3009675238866407</v>
-          </cell>
-          <cell r="T39">
-            <v>2.6394835897358155</v>
-          </cell>
-          <cell r="U39" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="V39" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="W39" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="X39" t="e">
-            <v>#N/A</v>
-          </cell>
-        </row>
-        <row r="40">
-          <cell r="G40">
-            <v>4.0999999999999996</v>
-          </cell>
-          <cell r="H40">
-            <v>7.8727010999999996</v>
-          </cell>
-          <cell r="I40">
-            <v>4.0999999999999996</v>
-          </cell>
-          <cell r="J40">
-            <v>5.0028286999999976</v>
-          </cell>
-          <cell r="K40">
-            <v>4.0999999999999996</v>
-          </cell>
-          <cell r="L40">
-            <v>5.3319650000000003</v>
-          </cell>
-          <cell r="M40">
-            <v>4.0999999999999996</v>
-          </cell>
-          <cell r="N40">
-            <v>5.6040891000000013</v>
-          </cell>
-          <cell r="P40">
-            <v>2.2789473684210528</v>
-          </cell>
-          <cell r="Q40">
-            <v>2.6954423812580237</v>
-          </cell>
-          <cell r="R40">
-            <v>2.6199218943517328</v>
-          </cell>
-          <cell r="S40">
-            <v>2.7832484530364385</v>
-          </cell>
-          <cell r="T40">
-            <v>3.2436648079144654</v>
-          </cell>
-          <cell r="U40" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="V40" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="W40" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="X40" t="e">
-            <v>#N/A</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="G41">
-            <v>4.2</v>
-          </cell>
-          <cell r="H41">
-            <v>8.3927928000000023</v>
-          </cell>
-          <cell r="I41">
-            <v>4.2</v>
-          </cell>
-          <cell r="J41">
-            <v>5.1411343609756086</v>
-          </cell>
-          <cell r="K41">
-            <v>4.2</v>
-          </cell>
-          <cell r="L41">
-            <v>5.4891746341463428</v>
-          </cell>
-          <cell r="M41">
-            <v>4.2</v>
-          </cell>
-          <cell r="N41">
-            <v>5.8948848000000016</v>
-          </cell>
-          <cell r="P41">
-            <v>2.642105263157895</v>
-          </cell>
-          <cell r="Q41">
-            <v>3.1870548395378697</v>
-          </cell>
-          <cell r="R41">
-            <v>3.0746395758664953</v>
-          </cell>
-          <cell r="S41">
-            <v>3.3089545263157909</v>
-          </cell>
-          <cell r="T41">
-            <v>3.8846179087076003</v>
-          </cell>
-          <cell r="U41" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="V41" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="W41" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="X41" t="e">
-            <v>#N/A</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="G42">
-            <v>4.3</v>
-          </cell>
-          <cell r="H42">
-            <v>8.9463176999999998</v>
-          </cell>
-          <cell r="I42">
-            <v>4.3</v>
-          </cell>
-          <cell r="J42">
-            <v>5.2802155195121934</v>
-          </cell>
-          <cell r="K42">
-            <v>4.3</v>
-          </cell>
-          <cell r="L42">
-            <v>5.6476776829268296</v>
-          </cell>
-          <cell r="M42">
-            <v>4.3</v>
-          </cell>
-          <cell r="N42">
-            <v>6.2108296999999988</v>
-          </cell>
-          <cell r="P42">
-            <v>3.0052631578947371</v>
-          </cell>
-          <cell r="Q42">
-            <v>3.6955497625160465</v>
-          </cell>
-          <cell r="R42">
-            <v>3.5394795413350448</v>
-          </cell>
-          <cell r="S42">
-            <v>4.0152335842105282</v>
-          </cell>
-          <cell r="T42">
-            <v>4.6593717166188142</v>
-          </cell>
-          <cell r="U42" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="V42" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="W42" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="X42" t="e">
-            <v>#N/A</v>
-          </cell>
-        </row>
-        <row r="43">
-          <cell r="G43">
-            <v>4.4000000000000004</v>
-          </cell>
-          <cell r="H43">
-            <v>9.5345184000000067</v>
-          </cell>
-          <cell r="I43">
-            <v>4.4000000000000004</v>
-          </cell>
-          <cell r="J43">
-            <v>5.4200721756097545</v>
-          </cell>
-          <cell r="K43">
-            <v>4.4000000000000004</v>
-          </cell>
-          <cell r="L43">
-            <v>5.8074741463414643</v>
-          </cell>
-          <cell r="M43">
-            <v>4.4000000000000004</v>
-          </cell>
-          <cell r="N43">
-            <v>6.5531663999999994</v>
-          </cell>
-          <cell r="P43">
-            <v>3.3684210526315792</v>
-          </cell>
-          <cell r="Q43">
-            <v>4.2213355969191282</v>
-          </cell>
-          <cell r="R43">
-            <v>4.0146866847240048</v>
-          </cell>
-          <cell r="S43">
-            <v>4.9699073368421054</v>
-          </cell>
-          <cell r="T43">
-            <v>5.9622935303505429</v>
-          </cell>
-          <cell r="U43" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="V43" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="W43" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="X43" t="e">
-            <v>#N/A</v>
-          </cell>
-        </row>
-        <row r="44">
-          <cell r="G44">
-            <v>4.5</v>
-          </cell>
-          <cell r="H44">
-            <v>10.158637500000005</v>
-          </cell>
-          <cell r="I44">
-            <v>4.5</v>
-          </cell>
-          <cell r="J44">
-            <v>5.5607043292682912</v>
-          </cell>
-          <cell r="K44">
-            <v>4.5</v>
-          </cell>
-          <cell r="L44">
-            <v>5.9685640243902451</v>
-          </cell>
-          <cell r="M44">
-            <v>4.5</v>
-          </cell>
-          <cell r="N44">
-            <v>6.9231375000000011</v>
-          </cell>
-          <cell r="P44">
-            <v>3.7315789473684213</v>
-          </cell>
-          <cell r="Q44">
-            <v>4.7640719704749692</v>
-          </cell>
-          <cell r="R44">
-            <v>4.5000569277278553</v>
-          </cell>
-          <cell r="S44">
-            <v>6.2277463736842122</v>
-          </cell>
-          <cell r="T44">
-            <v>8.0458957376154565</v>
-          </cell>
-          <cell r="U44" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="V44" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="W44" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="X44" t="e">
-            <v>#N/A</v>
-          </cell>
-        </row>
-        <row r="45">
-          <cell r="I45">
-            <v>4.5999999999999996</v>
-          </cell>
-          <cell r="J45">
-            <v>5.7021119804878024</v>
-          </cell>
-          <cell r="K45">
-            <v>4.5999999999999996</v>
-          </cell>
-          <cell r="L45">
-            <v>6.1309473170731712</v>
-          </cell>
-          <cell r="M45">
-            <v>4.5999999999999996</v>
-          </cell>
-          <cell r="N45">
-            <v>7.3219856000000005</v>
-          </cell>
-          <cell r="P45">
-            <v>4.094736842105263</v>
-          </cell>
-          <cell r="Q45">
-            <v>5.3237588831835696</v>
-          </cell>
-          <cell r="R45">
-            <v>4.9955902703465958</v>
-          </cell>
-          <cell r="S45">
-            <v>7.8470220947368423</v>
-          </cell>
-          <cell r="T45">
-            <v>11.187133579502049</v>
-          </cell>
-          <cell r="U45" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="V45" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="W45" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="X45">
-            <v>11.187133579502049</v>
-          </cell>
-        </row>
-        <row r="46">
-          <cell r="I46">
-            <v>4.7</v>
-          </cell>
-          <cell r="J46">
-            <v>5.844295129268291</v>
-          </cell>
-          <cell r="K46">
-            <v>4.7</v>
-          </cell>
-          <cell r="L46">
-            <v>6.294624024390246</v>
-          </cell>
-          <cell r="M46">
-            <v>4.7</v>
-          </cell>
-          <cell r="N46">
-            <v>7.7509533000000008</v>
-          </cell>
-          <cell r="P46">
-            <v>4.4578947368421051</v>
-          </cell>
-          <cell r="Q46">
-            <v>5.9007367073170736</v>
-          </cell>
-          <cell r="R46">
-            <v>5.5014907908857493</v>
-          </cell>
-          <cell r="S46">
-            <v>9.8958505105263193</v>
-          </cell>
-          <cell r="T46" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="U46" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="V46" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="W46">
-            <v>9.8958505105263193</v>
-          </cell>
-          <cell r="X46" t="e">
-            <v>#N/A</v>
-          </cell>
-        </row>
-        <row r="47">
-          <cell r="I47">
-            <v>4.8</v>
-          </cell>
-          <cell r="J47">
-            <v>5.9872537756097541</v>
-          </cell>
-          <cell r="K47">
-            <v>4.8</v>
-          </cell>
-          <cell r="L47">
-            <v>6.4595941463414634</v>
-          </cell>
-          <cell r="M47">
-            <v>4.8</v>
-          </cell>
-          <cell r="N47">
-            <v>8.2112832000000004</v>
-          </cell>
-          <cell r="P47">
-            <v>4.8210526315789473</v>
-          </cell>
-          <cell r="Q47">
-            <v>6.4945969961489096</v>
-          </cell>
-          <cell r="R47">
-            <v>6.0175135953786887</v>
-          </cell>
-          <cell r="S47" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="T47" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="U47" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="V47" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="W47" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="X47" t="e">
-            <v>#N/A</v>
-          </cell>
-        </row>
-        <row r="48">
-          <cell r="I48">
-            <v>4.9000000000000004</v>
-          </cell>
-          <cell r="J48">
-            <v>6.1309879195121937</v>
-          </cell>
-          <cell r="K48">
-            <v>4.9000000000000004</v>
-          </cell>
-          <cell r="L48">
-            <v>6.6258576829268314</v>
-          </cell>
-          <cell r="M48">
-            <v>4.9000000000000004</v>
-          </cell>
-          <cell r="N48">
-            <v>8.7042179000000033</v>
-          </cell>
-          <cell r="P48">
-            <v>5.1842105263157894</v>
-          </cell>
-          <cell r="Q48">
-            <v>7.0966237368421075</v>
-          </cell>
-          <cell r="R48">
-            <v>6.5424390368421026</v>
-          </cell>
-          <cell r="S48" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="T48" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="U48" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="V48" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="W48" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="X48" t="e">
-            <v>#N/A</v>
-          </cell>
-        </row>
-        <row r="49">
-          <cell r="I49">
-            <v>5</v>
-          </cell>
-          <cell r="J49">
-            <v>6.275497560975607</v>
-          </cell>
-          <cell r="K49">
-            <v>5</v>
-          </cell>
-          <cell r="L49">
-            <v>6.7934146341463428</v>
-          </cell>
-          <cell r="M49">
-            <v>5</v>
-          </cell>
-          <cell r="N49">
-            <v>9.2310000000000016</v>
-          </cell>
-          <cell r="P49">
-            <v>5.5473684210526315</v>
-          </cell>
-          <cell r="Q49">
-            <v>7.7260573684210474</v>
-          </cell>
-          <cell r="R49">
-            <v>7.1119623052631527</v>
-          </cell>
-          <cell r="S49" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="T49" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="U49" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="V49" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="W49" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="X49" t="e">
-            <v>#N/A</v>
-          </cell>
-        </row>
-        <row r="50">
-          <cell r="I50">
-            <v>5.0999999999999996</v>
-          </cell>
-          <cell r="J50">
-            <v>6.4207826999999975</v>
-          </cell>
-          <cell r="K50">
-            <v>5.0999999999999996</v>
-          </cell>
-          <cell r="L50">
-            <v>6.9622650000000013</v>
-          </cell>
-          <cell r="M50">
-            <v>5.0999999999999996</v>
-          </cell>
-          <cell r="N50">
-            <v>9.7928721000000003</v>
-          </cell>
-          <cell r="P50">
-            <v>5.9105263157894736</v>
-          </cell>
-          <cell r="Q50">
-            <v>8.4481583684210477</v>
-          </cell>
-          <cell r="R50">
-            <v>7.7647933210526245</v>
-          </cell>
-          <cell r="S50" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="T50" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="U50" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="V50" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="W50" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="X50" t="e">
-            <v>#N/A</v>
-          </cell>
-        </row>
-        <row r="51">
-          <cell r="I51">
-            <v>5.2</v>
-          </cell>
-          <cell r="J51">
-            <v>6.5652495999999978</v>
-          </cell>
-          <cell r="K51">
-            <v>5.2</v>
-          </cell>
-          <cell r="L51">
-            <v>7.1218160000000026</v>
-          </cell>
-          <cell r="M51">
-            <v>5.2</v>
-          </cell>
-          <cell r="N51">
-            <v>10.391076800000004</v>
-          </cell>
-          <cell r="P51">
-            <v>6.2736842105263158</v>
-          </cell>
-          <cell r="Q51">
-            <v>9.2789946315789393</v>
-          </cell>
-          <cell r="R51">
-            <v>8.5155651894736764</v>
-          </cell>
-          <cell r="S51" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="T51" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="U51" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="V51" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="W51" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="X51" t="e">
-            <v>#N/A</v>
-          </cell>
-        </row>
-        <row r="52">
-          <cell r="I52">
-            <v>5.3</v>
-          </cell>
-          <cell r="J52">
-            <v>6.7151688999999983</v>
-          </cell>
-          <cell r="K52">
-            <v>5.3</v>
-          </cell>
-          <cell r="L52">
-            <v>7.287447000000002</v>
-          </cell>
-          <cell r="M52">
-            <v>5.3</v>
-          </cell>
-          <cell r="N52">
-            <v>11.0268567</v>
-          </cell>
-          <cell r="P52">
-            <v>6.6368421052631579</v>
-          </cell>
-          <cell r="Q52">
-            <v>10.231455105263148</v>
-          </cell>
-          <cell r="R52">
-            <v>9.3760506368420931</v>
-          </cell>
-          <cell r="S52" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="T52" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="U52" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="V52" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="W52" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="X52" t="e">
-            <v>#N/A</v>
-          </cell>
-        </row>
-        <row r="53">
-          <cell r="I53">
-            <v>5.4</v>
-          </cell>
-          <cell r="J53">
-            <v>6.8708087999999981</v>
-          </cell>
-          <cell r="K53">
-            <v>5.4</v>
-          </cell>
-          <cell r="L53">
-            <v>7.4594520000000033</v>
-          </cell>
-          <cell r="M53">
-            <v>5.4</v>
-          </cell>
-          <cell r="N53">
-            <v>11.701454400000008</v>
-          </cell>
-          <cell r="P53">
-            <v>7</v>
-          </cell>
-          <cell r="Q53">
-            <v>11.318299999999986</v>
-          </cell>
-          <cell r="R53">
-            <v>10.357899999999985</v>
-          </cell>
-          <cell r="S53" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="T53" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="U53">
-            <v>11.318299999999986</v>
-          </cell>
-          <cell r="V53">
-            <v>10.357899999999985</v>
-          </cell>
-          <cell r="W53" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="X53" t="e">
-            <v>#N/A</v>
-          </cell>
-        </row>
-        <row r="54">
-          <cell r="I54">
-            <v>5.5</v>
-          </cell>
-          <cell r="J54">
-            <v>7.0324374999999968</v>
-          </cell>
-          <cell r="K54">
-            <v>5.5</v>
-          </cell>
-          <cell r="L54">
-            <v>7.6381249999999952</v>
-          </cell>
-          <cell r="M54">
-            <v>5.5</v>
-          </cell>
-          <cell r="N54">
-            <v>12.416112500000008</v>
-          </cell>
-        </row>
-        <row r="55">
-          <cell r="I55">
-            <v>5.6</v>
-          </cell>
-          <cell r="J55">
-            <v>7.2003231999999926</v>
-          </cell>
-          <cell r="K55">
-            <v>5.6</v>
-          </cell>
-          <cell r="L55">
-            <v>7.8237599999999947</v>
-          </cell>
-        </row>
-        <row r="56">
-          <cell r="I56">
-            <v>5.7</v>
-          </cell>
-          <cell r="J56">
-            <v>7.3747340999999915</v>
-          </cell>
-          <cell r="K56">
-            <v>5.7</v>
-          </cell>
-          <cell r="L56">
-            <v>8.016650999999996</v>
-          </cell>
-        </row>
-        <row r="57">
-          <cell r="I57">
-            <v>5.8</v>
-          </cell>
-          <cell r="J57">
-            <v>7.5559383999999934</v>
-          </cell>
-          <cell r="K57">
-            <v>5.8</v>
-          </cell>
-          <cell r="L57">
-            <v>8.2170919999999938</v>
-          </cell>
-        </row>
-        <row r="58">
-          <cell r="I58">
-            <v>5.9</v>
-          </cell>
-          <cell r="J58">
-            <v>7.7442042999999936</v>
-          </cell>
-          <cell r="K58">
-            <v>5.9</v>
-          </cell>
-          <cell r="L58">
-            <v>8.4253769999999957</v>
-          </cell>
-        </row>
-        <row r="59">
-          <cell r="I59">
-            <v>6</v>
-          </cell>
-          <cell r="J59">
-            <v>7.9397999999999929</v>
-          </cell>
-          <cell r="K59">
-            <v>6</v>
-          </cell>
-          <cell r="L59">
-            <v>8.6417999999999928</v>
-          </cell>
-        </row>
-        <row r="60">
-          <cell r="I60">
-            <v>6.1</v>
-          </cell>
-          <cell r="J60">
-            <v>8.1429936999999892</v>
-          </cell>
-          <cell r="K60">
-            <v>6.1</v>
-          </cell>
-          <cell r="L60">
-            <v>8.8666549999999908</v>
-          </cell>
-        </row>
-        <row r="61">
-          <cell r="I61">
-            <v>6.2</v>
-          </cell>
-          <cell r="J61">
-            <v>8.3540535999999932</v>
-          </cell>
-          <cell r="K61">
-            <v>6.2</v>
-          </cell>
-          <cell r="L61">
-            <v>9.1002359999999936</v>
-          </cell>
-        </row>
-        <row r="62">
-          <cell r="I62">
-            <v>6.3</v>
-          </cell>
-          <cell r="J62">
-            <v>8.5732478999999913</v>
-          </cell>
-          <cell r="K62">
-            <v>6.3</v>
-          </cell>
-          <cell r="L62">
-            <v>9.3428369999999923</v>
-          </cell>
-        </row>
-        <row r="63">
-          <cell r="I63">
-            <v>6.4</v>
-          </cell>
-          <cell r="J63">
-            <v>8.8008447999999895</v>
-          </cell>
-          <cell r="K63">
-            <v>6.4</v>
-          </cell>
-          <cell r="L63">
-            <v>9.5947519999999926</v>
-          </cell>
-        </row>
-        <row r="64">
-          <cell r="I64">
-            <v>6.5</v>
-          </cell>
-          <cell r="J64">
-            <v>9.0371124999999886</v>
-          </cell>
-          <cell r="K64">
-            <v>6.5</v>
-          </cell>
-          <cell r="L64">
-            <v>9.8562749999999895</v>
-          </cell>
-        </row>
-        <row r="65">
-          <cell r="I65">
-            <v>6.6</v>
-          </cell>
-          <cell r="J65">
-            <v>9.2823191999999874</v>
-          </cell>
-          <cell r="K65">
-            <v>6.6</v>
-          </cell>
-          <cell r="L65">
-            <v>10.127699999999988</v>
-          </cell>
-        </row>
-        <row r="66">
-          <cell r="I66">
-            <v>6.7</v>
-          </cell>
-          <cell r="J66">
-            <v>9.5367330999999886</v>
-          </cell>
-          <cell r="K66">
-            <v>6.7</v>
-          </cell>
-          <cell r="L66">
-            <v>10.40932099999999</v>
-          </cell>
-        </row>
-        <row r="67">
-          <cell r="I67">
-            <v>6.8</v>
-          </cell>
-          <cell r="J67">
-            <v>9.8006223999999857</v>
-          </cell>
-          <cell r="K67">
-            <v>6.8</v>
-          </cell>
-          <cell r="L67">
-            <v>10.701431999999986</v>
-          </cell>
-        </row>
-        <row r="68">
-          <cell r="I68">
-            <v>6.9</v>
-          </cell>
-          <cell r="J68">
-            <v>10.074255299999983</v>
-          </cell>
-          <cell r="K68">
-            <v>6.9</v>
-          </cell>
-          <cell r="L68">
-            <v>11.004326999999988</v>
-          </cell>
-        </row>
-        <row r="69">
-          <cell r="I69">
-            <v>7</v>
-          </cell>
-          <cell r="J69">
-            <v>10.357899999999985</v>
-          </cell>
-          <cell r="K69">
-            <v>7</v>
-          </cell>
-          <cell r="L69">
-            <v>11.318299999999986</v>
-          </cell>
-        </row>
-        <row r="70">
-          <cell r="I70">
-            <v>7.1</v>
-          </cell>
-          <cell r="J70">
-            <v>10.651824699999981</v>
-          </cell>
-          <cell r="K70">
-            <v>7.1</v>
-          </cell>
-          <cell r="L70">
-            <v>11.643644999999982</v>
-          </cell>
-        </row>
-        <row r="71">
-          <cell r="I71">
-            <v>7.2</v>
-          </cell>
-          <cell r="J71">
-            <v>10.956297599999981</v>
-          </cell>
-          <cell r="K71">
-            <v>7.2</v>
-          </cell>
-          <cell r="L71">
-            <v>11.980655999999982</v>
-          </cell>
-        </row>
-        <row r="72">
-          <cell r="I72">
-            <v>7.3</v>
-          </cell>
-          <cell r="J72">
-            <v>11.271586899999981</v>
-          </cell>
-          <cell r="K72">
-            <v>7.3</v>
-          </cell>
-          <cell r="L72">
-            <v>12.329626999999983</v>
-          </cell>
-        </row>
-        <row r="73">
-          <cell r="I73">
-            <v>7.4</v>
-          </cell>
-          <cell r="J73">
-            <v>11.59796079999998</v>
-          </cell>
-          <cell r="K73">
-            <v>7.4</v>
-          </cell>
-          <cell r="L73">
-            <v>12.690851999999982</v>
-          </cell>
-        </row>
-        <row r="74">
-          <cell r="I74">
-            <v>7.5</v>
-          </cell>
-          <cell r="J74">
-            <v>11.935687499999979</v>
-          </cell>
-          <cell r="K74">
-            <v>7.5</v>
-          </cell>
-          <cell r="L74">
-            <v>13.064624999999957</v>
-          </cell>
-        </row>
-        <row r="75">
-          <cell r="I75">
-            <v>7.6</v>
-          </cell>
-          <cell r="J75">
-            <v>12.28503519999998</v>
-          </cell>
-          <cell r="K75">
-            <v>7.6</v>
-          </cell>
-          <cell r="L75">
-            <v>13.451239999999958</v>
-          </cell>
-        </row>
-        <row r="76">
-          <cell r="I76">
-            <v>7.7</v>
-          </cell>
-          <cell r="J76">
-            <v>12.64627209999998</v>
-          </cell>
-          <cell r="K76">
-            <v>7.7</v>
-          </cell>
-          <cell r="L76">
-            <v>13.850990999999954</v>
-          </cell>
-        </row>
-        <row r="77">
-          <cell r="I77">
-            <v>7.8</v>
-          </cell>
-          <cell r="J77">
-            <v>13.019666399999975</v>
-          </cell>
-          <cell r="K77">
-            <v>7.8</v>
-          </cell>
-          <cell r="L77">
-            <v>14.264171999999952</v>
-          </cell>
-        </row>
-        <row r="78">
-          <cell r="I78">
-            <v>7.9</v>
-          </cell>
-          <cell r="J78">
-            <v>13.405486299999973</v>
-          </cell>
-          <cell r="K78">
-            <v>7.9</v>
-          </cell>
-          <cell r="L78">
-            <v>14.691076999999952</v>
-          </cell>
-        </row>
-        <row r="79">
-          <cell r="I79">
-            <v>8</v>
-          </cell>
-          <cell r="J79">
-            <v>13.803999999999972</v>
-          </cell>
-          <cell r="K79">
-            <v>8</v>
-          </cell>
-          <cell r="L79">
-            <v>15.131999999999948</v>
-          </cell>
-        </row>
-        <row r="80">
-          <cell r="I80">
-            <v>8.1</v>
-          </cell>
-          <cell r="J80">
-            <v>14.215475699999976</v>
-          </cell>
-          <cell r="K80">
-            <v>8.1</v>
-          </cell>
-          <cell r="L80">
-            <v>15.587234999999945</v>
-          </cell>
-        </row>
-        <row r="81">
-          <cell r="I81">
-            <v>8.1999999999999993</v>
-          </cell>
-          <cell r="J81">
-            <v>14.64018159999997</v>
-          </cell>
-          <cell r="K81">
-            <v>8.1999999999999993</v>
-          </cell>
-          <cell r="L81">
-            <v>16.057075999999942</v>
-          </cell>
-        </row>
-        <row r="82">
-          <cell r="I82">
-            <v>8.3000000000000007</v>
-          </cell>
-          <cell r="J82">
-            <v>15.078385899999942</v>
-          </cell>
-          <cell r="K82">
-            <v>8.3000000000000007</v>
-          </cell>
-          <cell r="L82">
-            <v>16.541816999999945</v>
-          </cell>
-        </row>
-        <row r="83">
-          <cell r="I83">
-            <v>8.4</v>
-          </cell>
-          <cell r="J83">
-            <v>15.530356799999943</v>
-          </cell>
-          <cell r="K83">
-            <v>8.4</v>
-          </cell>
-          <cell r="L83">
-            <v>17.041751999999942</v>
-          </cell>
-        </row>
-        <row r="84">
-          <cell r="I84">
-            <v>8.5</v>
-          </cell>
-          <cell r="J84">
-            <v>15.99636249999994</v>
-          </cell>
-          <cell r="K84">
-            <v>8.5</v>
-          </cell>
-          <cell r="L84">
-            <v>17.557174999999965</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="7"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Revision-History"/>
       <sheetName val="Data-Dictionary"/>
@@ -24744,6 +22425,189 @@
       </sheetData>
       <sheetData sheetId="9"/>
       <sheetData sheetId="10" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="DeviceCurrents"/>
+      <sheetName val="Revision-History"/>
+      <sheetName val="Data-Dictionary"/>
+      <sheetName val="Example-Pivot"/>
+      <sheetName val="Rechargeable-SOCs"/>
+      <sheetName val="Scenarios"/>
+      <sheetName val="Rayovac-Data"/>
+      <sheetName val="Logic"/>
+      <sheetName val="DeviceCurrentsCandidateTemp (2)"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4">
+        <row r="7">
+          <cell r="C7">
+            <v>0.8</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="5">
+        <row r="69">
+          <cell r="C69">
+            <v>0</v>
+          </cell>
+          <cell r="D69">
+            <v>3.5</v>
+          </cell>
+          <cell r="E69">
+            <v>0.16666666666666666</v>
+          </cell>
+          <cell r="F69">
+            <v>12.333333333333334</v>
+          </cell>
+          <cell r="H69">
+            <v>2700</v>
+          </cell>
+        </row>
+        <row r="70">
+          <cell r="C70">
+            <v>0.75</v>
+          </cell>
+          <cell r="D70">
+            <v>0</v>
+          </cell>
+          <cell r="E70">
+            <v>8.3333333333333329E-2</v>
+          </cell>
+          <cell r="F70">
+            <v>15.166666666666666</v>
+          </cell>
+          <cell r="H70">
+            <v>2430</v>
+          </cell>
+        </row>
+        <row r="71">
+          <cell r="C71">
+            <v>0</v>
+          </cell>
+          <cell r="D71">
+            <v>5</v>
+          </cell>
+          <cell r="E71">
+            <v>0.16666666666666666</v>
+          </cell>
+          <cell r="F71">
+            <v>12.833333333333332</v>
+          </cell>
+          <cell r="H71">
+            <v>1470</v>
+          </cell>
+        </row>
+        <row r="72">
+          <cell r="C72">
+            <v>1.5</v>
+          </cell>
+          <cell r="D72">
+            <v>0</v>
+          </cell>
+          <cell r="E72">
+            <v>8.3333333333333329E-2</v>
+          </cell>
+          <cell r="F72">
+            <v>16.416666666666668</v>
+          </cell>
+          <cell r="H72">
+            <v>1380</v>
+          </cell>
+        </row>
+        <row r="73">
+          <cell r="C73">
+            <v>13.833333333333334</v>
+          </cell>
+          <cell r="D73">
+            <v>0</v>
+          </cell>
+          <cell r="E73">
+            <v>0.16666666666666666</v>
+          </cell>
+          <cell r="F73">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="74">
+          <cell r="C74">
+            <v>15.833333333333334</v>
+          </cell>
+          <cell r="D74">
+            <v>0</v>
+          </cell>
+          <cell r="E74">
+            <v>0.16666666666666666</v>
+          </cell>
+          <cell r="F74">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="75">
+          <cell r="C75">
+            <v>0</v>
+          </cell>
+          <cell r="D75">
+            <v>3.5</v>
+          </cell>
+          <cell r="E75">
+            <v>0.16666666666666666</v>
+          </cell>
+          <cell r="F75">
+            <v>12.333333333333334</v>
+          </cell>
+        </row>
+        <row r="76">
+          <cell r="C76">
+            <v>0</v>
+          </cell>
+          <cell r="D76">
+            <v>5</v>
+          </cell>
+          <cell r="E76">
+            <v>0.16666666666666666</v>
+          </cell>
+          <cell r="F76">
+            <v>12.833333333333332</v>
+          </cell>
+        </row>
+        <row r="77">
+          <cell r="C77">
+            <v>0</v>
+          </cell>
+          <cell r="D77">
+            <v>0</v>
+          </cell>
+          <cell r="E77">
+            <v>0</v>
+          </cell>
+          <cell r="F77">
+            <v>16</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="6">
+        <row r="2">
+          <cell r="Q2" t="str">
+            <v>Derating vs Actual Current and Size</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -25094,8 +22958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6C6117C-15EB-42A3-BAAC-821B7C414687}">
   <dimension ref="A2:AE242"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AA49" sqref="AA49"/>
+    <sheetView tabSelected="1" topLeftCell="P54" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="X71" sqref="X71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -28108,7 +25972,7 @@
         <v>9.8562749999999895</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>10</v>
       </c>
@@ -28135,7 +25999,7 @@
         <v>10.127699999999988</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>10</v>
       </c>
@@ -28162,7 +26026,7 @@
         <v>10.40932099999999</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>10</v>
       </c>
@@ -28189,7 +26053,7 @@
         <v>10.701431999999986</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>10</v>
       </c>
@@ -28216,7 +26080,7 @@
         <v>11.004326999999988</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>10</v>
       </c>
@@ -28243,7 +26107,7 @@
         <v>11.318299999999986</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>10</v>
       </c>
@@ -28270,7 +26134,7 @@
         <v>11.643644999999982</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>10</v>
       </c>
@@ -28297,7 +26161,7 @@
         <v>11.980655999999982</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>10</v>
       </c>
@@ -28323,8 +26187,11 @@
       <c r="L72" s="1">
         <v>12.329626999999983</v>
       </c>
+      <c r="Q72" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>10</v>
       </c>
@@ -28350,8 +26217,11 @@
       <c r="L73" s="1">
         <v>12.690851999999982</v>
       </c>
+      <c r="Q73" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>10</v>
       </c>
@@ -28378,7 +26248,7 @@
         <v>13.064624999999957</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>10</v>
       </c>
@@ -28405,7 +26275,7 @@
         <v>13.451239999999958</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>10</v>
       </c>
@@ -28432,7 +26302,7 @@
         <v>13.850990999999954</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>10</v>
       </c>
@@ -28459,7 +26329,7 @@
         <v>14.264171999999952</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>10</v>
       </c>
@@ -28486,7 +26356,7 @@
         <v>14.691076999999952</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>10</v>
       </c>
@@ -28513,7 +26383,7 @@
         <v>15.131999999999948</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>10</v>
       </c>

</xml_diff>